<commit_message>
finished procedurestuff mayebe, and made changes in schememini
</commit_message>
<xml_diff>
--- a/Horrific_Medusa_Excel/SchemaMini.xlsx
+++ b/Horrific_Medusa_Excel/SchemaMini.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="7">
   <si>
     <t xml:space="preserve">Available </t>
   </si>
@@ -32,16 +32,19 @@
     <t>ArtistID</t>
   </si>
   <si>
-    <t>StartTime</t>
-  </si>
-  <si>
-    <t>EndTime</t>
-  </si>
-  <si>
     <t>False</t>
   </si>
   <si>
     <t>True</t>
+  </si>
+  <si>
+    <t>SchemeStartDate</t>
+  </si>
+  <si>
+    <t>SchemeEndTime</t>
+  </si>
+  <si>
+    <t>ReservationID</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H27"/>
+  <dimension ref="B2:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,7 +409,7 @@
     <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -414,15 +417,18 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -433,10 +439,13 @@
       <c r="H4" s="1">
         <v>42688.395833333336</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -447,10 +456,13 @@
       <c r="H5" s="1">
         <v>42688.416666666664</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -462,9 +474,9 @@
         <v>42688.354166666664</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -476,9 +488,9 @@
         <v>42688.375</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -490,9 +502,9 @@
         <v>42689.375</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -504,9 +516,9 @@
         <v>42689.395833333336</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -517,10 +529,13 @@
       <c r="H11" s="1">
         <v>42689.395833333336</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -531,10 +546,13 @@
       <c r="H12" s="1">
         <v>42689.4375</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -545,10 +563,13 @@
       <c r="H14" s="1">
         <v>42690.375</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -559,10 +580,13 @@
       <c r="H15" s="1">
         <v>42690.395833333336</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -573,10 +597,13 @@
       <c r="H16" s="1">
         <v>42690.354166666664</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -587,10 +614,13 @@
       <c r="H17" s="1">
         <v>42690.375</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -602,9 +632,9 @@
         <v>42691.375</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -616,9 +646,9 @@
         <v>42691.395833333336</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -629,10 +659,13 @@
       <c r="H21" s="1">
         <v>42691.375</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D22">
         <v>3</v>
@@ -643,10 +676,13 @@
       <c r="H22" s="1">
         <v>42691.416666666664</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -657,10 +693,13 @@
       <c r="H24" s="1">
         <v>42692.395833333336</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -671,10 +710,13 @@
       <c r="H25" s="1">
         <v>42692.4375</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -685,10 +727,13 @@
       <c r="H26" s="1">
         <v>42692.416666666664</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -698,6 +743,9 @@
       </c>
       <c r="H27" s="1">
         <v>42692.458333333336</v>
+      </c>
+      <c r="J27">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added insert data mini scheme
</commit_message>
<xml_diff>
--- a/Horrific_Medusa_Excel/SchemaMini.xlsx
+++ b/Horrific_Medusa_Excel/SchemaMini.xlsx
@@ -397,354 +397,353 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J23"/>
+  <dimension ref="B1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>42688.375</v>
+      </c>
+      <c r="E2" s="1">
+        <v>42688.395833333336</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>42688.395833333336</v>
+      </c>
+      <c r="E3" s="1">
+        <v>42688.416666666664</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>42688.333333333336</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42688.354166666664</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>42688.354166666664</v>
+      </c>
+      <c r="E5" s="1">
         <v>42688.375</v>
       </c>
-      <c r="H4" s="1">
-        <v>42688.395833333336</v>
-      </c>
-      <c r="J4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1">
-        <v>42688.395833333336</v>
-      </c>
-      <c r="H5" s="1">
-        <v>42688.416666666664</v>
-      </c>
-      <c r="J5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="F6" s="1">
-        <v>42688.333333333336</v>
-      </c>
-      <c r="H6" s="1">
-        <v>42688.354166666664</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>42689.354166666664</v>
+      </c>
+      <c r="E6" s="1">
+        <v>42689.375</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="F7" s="1">
-        <v>42688.354166666664</v>
-      </c>
-      <c r="H7" s="1">
-        <v>42688.375</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>42689.375</v>
+      </c>
+      <c r="E7" s="1">
+        <v>42689.395833333336</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
         <v>42689.354166666664</v>
       </c>
-      <c r="H8" s="1">
-        <v>42689.375</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>42689.395833333336</v>
+      </c>
+      <c r="F8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="F9" s="1">
-        <v>42689.375</v>
-      </c>
-      <c r="H9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
         <v>42689.395833333336</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>42689.4375</v>
+      </c>
+      <c r="F9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="F10" s="1">
-        <v>42689.354166666664</v>
-      </c>
-      <c r="H10" s="1">
-        <v>42689.395833333336</v>
-      </c>
-      <c r="J10">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>42690.354166666664</v>
+      </c>
+      <c r="E10" s="1">
+        <v>42690.375</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="F11" s="1">
-        <v>42689.395833333336</v>
-      </c>
-      <c r="H11" s="1">
-        <v>42689.4375</v>
-      </c>
-      <c r="J11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>42690.375</v>
+      </c>
+      <c r="E11" s="1">
+        <v>42690.395833333336</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>2</v>
       </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>42690.333333333336</v>
+      </c>
+      <c r="E12" s="1">
         <v>42690.354166666664</v>
       </c>
-      <c r="H12" s="1">
+      <c r="F12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>42690.354166666664</v>
+      </c>
+      <c r="E13" s="1">
         <v>42690.375</v>
       </c>
-      <c r="J12">
+      <c r="F13">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="F13" s="1">
-        <v>42690.375</v>
-      </c>
-      <c r="H13" s="1">
-        <v>42690.395833333336</v>
-      </c>
-      <c r="J13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="F14" s="1">
-        <v>42690.333333333336</v>
-      </c>
-      <c r="H14" s="1">
-        <v>42690.354166666664</v>
-      </c>
-      <c r="J14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>42691.354166666664</v>
+      </c>
+      <c r="E14" s="1">
+        <v>42691.375</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="F15" s="1">
-        <v>42690.354166666664</v>
-      </c>
-      <c r="H15" s="1">
-        <v>42690.375</v>
-      </c>
-      <c r="J15">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>42691.375</v>
+      </c>
+      <c r="E15" s="1">
+        <v>42691.395833333336</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="F16" s="1">
-        <v>42691.354166666664</v>
-      </c>
-      <c r="H16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>42691.333333333336</v>
+      </c>
+      <c r="E16" s="1">
         <v>42691.375</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
         <v>42691.375</v>
       </c>
-      <c r="H17" s="1">
-        <v>42691.395833333336</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <v>42691.416666666664</v>
+      </c>
+      <c r="F17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>2</v>
       </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="F18" s="1">
-        <v>42691.333333333336</v>
-      </c>
-      <c r="H18" s="1">
-        <v>42691.375</v>
-      </c>
-      <c r="J18">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>42692.354166666664</v>
+      </c>
+      <c r="E18" s="1">
+        <v>42692.395833333336</v>
+      </c>
+      <c r="F18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>2</v>
       </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-      <c r="F19" s="1">
-        <v>42691.375</v>
-      </c>
-      <c r="H19" s="1">
-        <v>42691.416666666664</v>
-      </c>
-      <c r="J19">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>42692.395833333336</v>
+      </c>
+      <c r="E19" s="1">
+        <v>42692.4375</v>
+      </c>
+      <c r="F19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>2</v>
       </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="F20" s="1">
-        <v>42692.354166666664</v>
-      </c>
-      <c r="H20" s="1">
-        <v>42692.395833333336</v>
-      </c>
-      <c r="J20">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>42692.375</v>
+      </c>
+      <c r="E20" s="1">
+        <v>42692.416666666664</v>
+      </c>
+      <c r="F20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>2</v>
       </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="F21" s="1">
-        <v>42692.395833333336</v>
-      </c>
-      <c r="H21" s="1">
-        <v>42692.4375</v>
-      </c>
-      <c r="J21">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-      <c r="F22" s="1">
-        <v>42692.375</v>
-      </c>
-      <c r="H22" s="1">
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1">
         <v>42692.416666666664</v>
       </c>
-      <c r="J22">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="F23" s="1">
-        <v>42692.416666666664</v>
-      </c>
-      <c r="H23" s="1">
+      <c r="E21" s="1">
         <v>42692.458333333336</v>
       </c>
-      <c r="J23">
+      <c r="F21">
         <v>18</v>
       </c>
     </row>

</xml_diff>